<commit_message>
Add Adobe fonts for Simplified Chinese
</commit_message>
<xml_diff>
--- a/trans/initial_data/initial_data.xlsx
+++ b/trans/initial_data/initial_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamid/GitHub/translation/trans/initial_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanwentao/repo/ioi/translation/trans/initial_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563C5EC4-84B1-A042-B27B-982F37BBBFDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16180" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Languages" sheetId="3" r:id="rId3"/>
     <sheet name="Initial Data" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="387">
   <si>
     <t>Username</t>
   </si>
@@ -1167,16 +1168,52 @@
   </si>
   <si>
     <t>This sheet contains data imported separately by loaddata command, and is not used by initialize command.</t>
+  </si>
+  <si>
+    <t>zh-CN</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ltr</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>zh-TW</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>zh-HK</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>zh-MO</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Simplified Chinese</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Traditional Chinese</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Traditional Chinese, Hong Kong</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Traditional Chinese, Macao</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1199,7 +1236,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1213,6 +1250,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1259,7 +1307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1308,7 +1356,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1322,6 +1370,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1399,6 +1451,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1666,21 +1721,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
     <col min="5" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1694,7 +1749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1708,7 +1763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1722,7 +1777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1736,7 +1791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1750,7 +1805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1764,7 +1819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1778,7 +1833,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1792,7 +1847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1806,7 +1861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -1820,7 +1875,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -1834,7 +1889,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1848,7 +1903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -1862,7 +1917,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
@@ -1876,7 +1931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
@@ -1890,7 +1945,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1904,21 +1959,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>32</v>
+      <c r="C17" s="40" t="s">
+        <v>378</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -1932,7 +1987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -1946,7 +2001,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1960,7 +2015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1974,7 +2029,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
@@ -1988,7 +2043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -2002,7 +2057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
@@ -2016,7 +2071,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>42</v>
       </c>
@@ -2030,7 +2085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
@@ -2044,7 +2099,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
         <v>45</v>
       </c>
@@ -2058,7 +2113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>47</v>
       </c>
@@ -2072,7 +2127,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>49</v>
       </c>
@@ -2086,7 +2141,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>50</v>
       </c>
@@ -2100,7 +2155,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
@@ -2114,7 +2169,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>53</v>
       </c>
@@ -2128,21 +2183,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>10</v>
+      <c r="C33" s="40" t="s">
+        <v>381</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>55</v>
       </c>
@@ -2156,7 +2211,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
         <v>57</v>
       </c>
@@ -2170,7 +2225,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
         <v>59</v>
       </c>
@@ -2184,7 +2239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>60</v>
       </c>
@@ -2198,7 +2253,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
         <v>62</v>
       </c>
@@ -2212,7 +2267,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
         <v>64</v>
       </c>
@@ -2226,7 +2281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
         <v>65</v>
       </c>
@@ -2240,7 +2295,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
         <v>67</v>
       </c>
@@ -2254,7 +2309,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
         <v>69</v>
       </c>
@@ -2268,7 +2323,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
         <v>70</v>
       </c>
@@ -2282,7 +2337,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
         <v>72</v>
       </c>
@@ -2296,7 +2351,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>74</v>
       </c>
@@ -2310,7 +2365,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
         <v>75</v>
       </c>
@@ -2324,7 +2379,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
         <v>77</v>
       </c>
@@ -2338,21 +2393,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>27</v>
+      <c r="C48" s="40" t="s">
+        <v>382</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>79</v>
       </c>
@@ -2366,7 +2421,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>80</v>
       </c>
@@ -2380,7 +2435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
         <v>81</v>
       </c>
@@ -2394,7 +2449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>82</v>
       </c>
@@ -2408,7 +2463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>83</v>
       </c>
@@ -2422,7 +2477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
         <v>84</v>
       </c>
@@ -2436,7 +2491,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
         <v>85</v>
       </c>
@@ -2450,7 +2505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>86</v>
       </c>
@@ -2464,7 +2519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>87</v>
       </c>
@@ -2478,7 +2533,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>88</v>
       </c>
@@ -2492,7 +2547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
         <v>90</v>
       </c>
@@ -2506,7 +2561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
         <v>91</v>
       </c>
@@ -2520,7 +2575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
         <v>92</v>
       </c>
@@ -2534,7 +2589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>94</v>
       </c>
@@ -2548,7 +2603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
         <v>95</v>
       </c>
@@ -2562,7 +2617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
         <v>97</v>
       </c>
@@ -2576,7 +2631,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
         <v>99</v>
       </c>
@@ -2590,7 +2645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
         <v>101</v>
       </c>
@@ -2604,7 +2659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
         <v>103</v>
       </c>
@@ -2618,7 +2673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
         <v>104</v>
       </c>
@@ -2632,7 +2687,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
         <v>106</v>
       </c>
@@ -2646,7 +2701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
         <v>108</v>
       </c>
@@ -2660,7 +2715,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
         <v>109</v>
       </c>
@@ -2674,7 +2729,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
         <v>110</v>
       </c>
@@ -2688,7 +2743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
         <v>111</v>
       </c>
@@ -2702,7 +2757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
         <v>113</v>
       </c>
@@ -2716,7 +2771,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
         <v>114</v>
       </c>
@@ -2730,21 +2785,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>32</v>
+      <c r="C76" s="40" t="s">
+        <v>380</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
         <v>116</v>
       </c>
@@ -2758,7 +2813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
         <v>118</v>
       </c>
@@ -2772,7 +2827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
         <v>119</v>
       </c>
@@ -2786,7 +2841,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
         <v>120</v>
       </c>
@@ -2800,7 +2855,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
         <v>122</v>
       </c>
@@ -2814,7 +2869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
         <v>124</v>
       </c>
@@ -2828,7 +2883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
         <v>126</v>
       </c>
@@ -2842,7 +2897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
         <v>127</v>
       </c>
@@ -2856,7 +2911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
         <v>128</v>
       </c>
@@ -2870,7 +2925,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
         <v>130</v>
       </c>
@@ -2885,6 +2940,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -2895,17 +2951,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IV88"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="4" customWidth="1"/>
     <col min="2" max="3" width="12.5" style="4" customWidth="1"/>
@@ -2913,7 +2969,7 @@
     <col min="257" max="1025" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="8" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:256" s="8" customFormat="1" ht="14.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -3177,7 +3233,7 @@
       <c r="IU1" s="7"/>
       <c r="IV1" s="7"/>
     </row>
-    <row r="2" spans="1:256" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:256" ht="14.75" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>133</v>
       </c>
@@ -3188,7 +3244,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:256" ht="14.5" customHeight="1">
       <c r="A3" s="9" t="s">
         <v>135</v>
       </c>
@@ -3199,7 +3255,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:256" ht="14.5" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>137</v>
       </c>
@@ -3210,7 +3266,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:256" ht="14.5" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>139</v>
       </c>
@@ -3221,7 +3277,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:256" ht="14.5" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>141</v>
       </c>
@@ -3232,7 +3288,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:256" ht="14.5" customHeight="1">
       <c r="A7" s="9" t="s">
         <v>143</v>
       </c>
@@ -3243,7 +3299,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:256" ht="14.5" customHeight="1">
       <c r="A8" s="9" t="s">
         <v>145</v>
       </c>
@@ -3254,7 +3310,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:256" ht="14.5" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>147</v>
       </c>
@@ -3265,7 +3321,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:256" ht="14.5" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>149</v>
       </c>
@@ -3276,7 +3332,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:256" ht="14.5" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>151</v>
       </c>
@@ -3287,7 +3343,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="12" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:256" ht="14.5" customHeight="1">
       <c r="A12" s="9" t="s">
         <v>153</v>
       </c>
@@ -3298,7 +3354,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:256" ht="14.5" customHeight="1">
       <c r="A13" s="9" t="s">
         <v>155</v>
       </c>
@@ -3309,7 +3365,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:256" ht="14.5" customHeight="1">
       <c r="A14" s="9" t="s">
         <v>157</v>
       </c>
@@ -3320,7 +3376,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:256" ht="14.5" customHeight="1">
       <c r="A15" s="9" t="s">
         <v>159</v>
       </c>
@@ -3331,7 +3387,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:256" ht="14.5" customHeight="1">
       <c r="A16" s="9" t="s">
         <v>161</v>
       </c>
@@ -3342,7 +3398,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="14.5" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>163</v>
       </c>
@@ -3353,7 +3409,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="14.5" customHeight="1">
       <c r="A18" s="9" t="s">
         <v>165</v>
       </c>
@@ -3364,7 +3420,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="14.5" customHeight="1">
       <c r="A19" s="9" t="s">
         <v>167</v>
       </c>
@@ -3375,7 +3431,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="14.5" customHeight="1">
       <c r="A20" s="9" t="s">
         <v>169</v>
       </c>
@@ -3386,7 +3442,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="14.5" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>171</v>
       </c>
@@ -3397,7 +3453,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="14.5" customHeight="1">
       <c r="A22" s="9" t="s">
         <v>173</v>
       </c>
@@ -3408,7 +3464,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="14.5" customHeight="1">
       <c r="A23" s="9" t="s">
         <v>175</v>
       </c>
@@ -3419,7 +3475,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="14.5" customHeight="1">
       <c r="A24" s="9" t="s">
         <v>177</v>
       </c>
@@ -3430,7 +3486,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="14.5" customHeight="1">
       <c r="A25" s="9" t="s">
         <v>179</v>
       </c>
@@ -3441,7 +3497,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="14.5" customHeight="1">
       <c r="A26" s="9" t="s">
         <v>181</v>
       </c>
@@ -3452,7 +3508,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="14.5" customHeight="1">
       <c r="A27" s="9" t="s">
         <v>183</v>
       </c>
@@ -3463,7 +3519,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="14.5" customHeight="1">
       <c r="A28" s="9" t="s">
         <v>185</v>
       </c>
@@ -3474,7 +3530,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="14.5" customHeight="1">
       <c r="A29" s="9" t="s">
         <v>187</v>
       </c>
@@ -3485,7 +3541,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="14.5" customHeight="1">
       <c r="A30" s="9" t="s">
         <v>189</v>
       </c>
@@ -3496,7 +3552,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="14.5" customHeight="1">
       <c r="A31" s="9" t="s">
         <v>191</v>
       </c>
@@ -3507,7 +3563,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="14.5" customHeight="1">
       <c r="A32" s="9" t="s">
         <v>193</v>
       </c>
@@ -3518,7 +3574,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="14.5" customHeight="1">
       <c r="A33" s="9" t="s">
         <v>195</v>
       </c>
@@ -3529,7 +3585,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="14.5" customHeight="1">
       <c r="A34" s="9" t="s">
         <v>197</v>
       </c>
@@ -3540,7 +3596,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="14.5" customHeight="1">
       <c r="A35" s="9" t="s">
         <v>199</v>
       </c>
@@ -3551,7 +3607,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="14.5" customHeight="1">
       <c r="A36" s="9" t="s">
         <v>201</v>
       </c>
@@ -3562,7 +3618,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="14.5" customHeight="1">
       <c r="A37" s="9" t="s">
         <v>203</v>
       </c>
@@ -3573,7 +3629,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="14.5" customHeight="1">
       <c r="A38" s="9" t="s">
         <v>205</v>
       </c>
@@ -3584,7 +3640,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="14.5" customHeight="1">
       <c r="A39" s="9" t="s">
         <v>207</v>
       </c>
@@ -3595,7 +3651,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="14.5" customHeight="1">
       <c r="A40" s="9" t="s">
         <v>209</v>
       </c>
@@ -3606,7 +3662,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="14.5" customHeight="1">
       <c r="A41" s="9" t="s">
         <v>211</v>
       </c>
@@ -3617,7 +3673,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="14.5" customHeight="1">
       <c r="A42" s="9" t="s">
         <v>213</v>
       </c>
@@ -3628,7 +3684,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="14.5" customHeight="1">
       <c r="A43" s="9" t="s">
         <v>215</v>
       </c>
@@ -3639,7 +3695,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="14.5" customHeight="1">
       <c r="A44" s="9" t="s">
         <v>217</v>
       </c>
@@ -3650,7 +3706,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="14.5" customHeight="1">
       <c r="A45" s="9" t="s">
         <v>219</v>
       </c>
@@ -3661,7 +3717,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="14.5" customHeight="1">
       <c r="A46" s="9" t="s">
         <v>221</v>
       </c>
@@ -3672,7 +3728,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="14.5" customHeight="1">
       <c r="A47" s="9" t="s">
         <v>223</v>
       </c>
@@ -3683,7 +3739,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="14.5" customHeight="1">
       <c r="A48" s="9" t="s">
         <v>225</v>
       </c>
@@ -3694,7 +3750,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="14.5" customHeight="1">
       <c r="A49" s="9" t="s">
         <v>227</v>
       </c>
@@ -3705,7 +3761,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="14.5" customHeight="1">
       <c r="A50" s="9" t="s">
         <v>229</v>
       </c>
@@ -3716,7 +3772,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="14.5" customHeight="1">
       <c r="A51" s="9" t="s">
         <v>231</v>
       </c>
@@ -3727,7 +3783,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="14.5" customHeight="1">
       <c r="A52" s="9" t="s">
         <v>233</v>
       </c>
@@ -3738,7 +3794,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="14.5" customHeight="1">
       <c r="A53" s="9" t="s">
         <v>235</v>
       </c>
@@ -3749,7 +3805,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="14.5" customHeight="1">
       <c r="A54" s="9" t="s">
         <v>237</v>
       </c>
@@ -3760,7 +3816,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="14.5" customHeight="1">
       <c r="A55" s="9" t="s">
         <v>239</v>
       </c>
@@ -3771,7 +3827,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="14.5" customHeight="1">
       <c r="A56" s="9" t="s">
         <v>241</v>
       </c>
@@ -3782,7 +3838,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="14.5" customHeight="1">
       <c r="A57" s="9" t="s">
         <v>243</v>
       </c>
@@ -3793,7 +3849,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" ht="14.5" customHeight="1">
       <c r="A58" s="9" t="s">
         <v>245</v>
       </c>
@@ -3804,7 +3860,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="14.5" customHeight="1">
       <c r="A59" s="9" t="s">
         <v>247</v>
       </c>
@@ -3815,7 +3871,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" ht="14.5" customHeight="1">
       <c r="A60" s="9" t="s">
         <v>249</v>
       </c>
@@ -3826,7 +3882,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" ht="14.5" customHeight="1">
       <c r="A61" s="9" t="s">
         <v>251</v>
       </c>
@@ -3837,7 +3893,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" ht="14.5" customHeight="1">
       <c r="A62" s="9" t="s">
         <v>253</v>
       </c>
@@ -3848,7 +3904,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="14.5" customHeight="1">
       <c r="A63" s="9" t="s">
         <v>255</v>
       </c>
@@ -3859,7 +3915,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" ht="14.5" customHeight="1">
       <c r="A64" s="9" t="s">
         <v>257</v>
       </c>
@@ -3870,7 +3926,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" ht="14.5" customHeight="1">
       <c r="A65" s="9" t="s">
         <v>259</v>
       </c>
@@ -3881,7 +3937,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" ht="14.5" customHeight="1">
       <c r="A66" s="9" t="s">
         <v>261</v>
       </c>
@@ -3892,7 +3948,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" ht="14.5" customHeight="1">
       <c r="A67" s="9" t="s">
         <v>263</v>
       </c>
@@ -3903,7 +3959,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" ht="14.5" customHeight="1">
       <c r="A68" s="9" t="s">
         <v>265</v>
       </c>
@@ -3914,7 +3970,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="14.5" customHeight="1">
       <c r="A69" s="9" t="s">
         <v>267</v>
       </c>
@@ -3925,7 +3981,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" ht="14.5" customHeight="1">
       <c r="A70" s="9" t="s">
         <v>269</v>
       </c>
@@ -3936,7 +3992,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="14.5" customHeight="1">
       <c r="A71" s="9" t="s">
         <v>271</v>
       </c>
@@ -3947,7 +4003,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="14.5" customHeight="1">
       <c r="A72" s="9" t="s">
         <v>273</v>
       </c>
@@ -3958,7 +4014,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" ht="14.5" customHeight="1">
       <c r="A73" s="9" t="s">
         <v>275</v>
       </c>
@@ -3969,7 +4025,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="14.5" customHeight="1">
       <c r="A74" s="9" t="s">
         <v>277</v>
       </c>
@@ -3980,7 +4036,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="14.5" customHeight="1">
       <c r="A75" s="9" t="s">
         <v>279</v>
       </c>
@@ -3991,7 +4047,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" ht="14.5" customHeight="1">
       <c r="A76" s="9" t="s">
         <v>281</v>
       </c>
@@ -4002,7 +4058,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" ht="14.5" customHeight="1">
       <c r="A77" s="9" t="s">
         <v>283</v>
       </c>
@@ -4013,7 +4069,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="14.5" customHeight="1">
       <c r="A78" s="9" t="s">
         <v>285</v>
       </c>
@@ -4024,7 +4080,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" ht="14.5" customHeight="1">
       <c r="A79" s="9" t="s">
         <v>287</v>
       </c>
@@ -4035,7 +4091,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="14.5" customHeight="1">
       <c r="A80" s="9" t="s">
         <v>289</v>
       </c>
@@ -4046,7 +4102,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="14.5" customHeight="1">
       <c r="A81" s="9" t="s">
         <v>291</v>
       </c>
@@ -4057,7 +4113,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="14.5" customHeight="1">
       <c r="A82" s="9" t="s">
         <v>293</v>
       </c>
@@ -4068,7 +4124,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="14.5" customHeight="1">
       <c r="A83" s="9" t="s">
         <v>295</v>
       </c>
@@ -4079,7 +4135,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="14.5" customHeight="1">
       <c r="A84" s="9" t="s">
         <v>297</v>
       </c>
@@ -4090,7 +4146,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="14.5" customHeight="1">
       <c r="A85" s="9" t="s">
         <v>299</v>
       </c>
@@ -4101,10 +4157,11 @@
         <v>300</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" spans="1:3" ht="14.5" customHeight="1"/>
+    <row r="87" spans="1:3" ht="14.5" customHeight="1"/>
+    <row r="88" spans="1:3" ht="14.5" customHeight="1"/>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -4114,26 +4171,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV43"/>
+  <dimension ref="A1:IV47"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B28" activeCellId="1" sqref="C62 B28"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="27" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" style="4" customWidth="1"/>
     <col min="4" max="256" width="16.33203125" style="4" customWidth="1"/>
     <col min="257" max="1025" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="8" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:256" s="8" customFormat="1" ht="14.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -4397,7 +4454,7 @@
       <c r="IU1" s="7"/>
       <c r="IV1" s="7"/>
     </row>
-    <row r="2" spans="1:256" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:256" ht="14.75" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>302</v>
       </c>
@@ -4408,7 +4465,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:256" ht="14.5" customHeight="1">
       <c r="A3" s="9" t="s">
         <v>304</v>
       </c>
@@ -4419,7 +4476,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="4" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:256" ht="14.5" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>306</v>
       </c>
@@ -4430,7 +4487,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="5" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:256" ht="14.5" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>307</v>
       </c>
@@ -4441,7 +4498,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="6" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:256" ht="14.5" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>308</v>
       </c>
@@ -4452,7 +4509,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="7" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:256" ht="14.5" customHeight="1">
       <c r="A7" s="9" t="s">
         <v>309</v>
       </c>
@@ -4463,403 +4520,448 @@
         <v>305</v>
       </c>
     </row>
-    <row r="8" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:256" ht="14.5" customHeight="1">
+      <c r="A8" s="41" t="s">
+        <v>383</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>378</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="9" spans="1:256" ht="14.5" customHeight="1">
+      <c r="A9" s="41" t="s">
+        <v>384</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>380</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="10" spans="1:256" ht="14.5" customHeight="1">
+      <c r="A10" s="41" t="s">
+        <v>385</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>381</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="11" spans="1:256" ht="14.5" customHeight="1">
+      <c r="A11" s="41" t="s">
+        <v>386</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>382</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:256" ht="14.5" customHeight="1">
+      <c r="A12" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="9" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="10" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="11" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="12" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="13" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:256" ht="14.5" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="14" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:256" ht="14.5" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="15" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:256" ht="14.5" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="16" spans="1:256" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:256" ht="14.5" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="14.5" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>320</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.5" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="14.5" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="14.5" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="14.5" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>68</v>
+        <v>320</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.5" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="14.5" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="14.5" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="14.5" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="14.5" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.5" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="14.5" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="14.5" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="14.5" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.5" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="14.5" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="14.5" customHeight="1">
       <c r="A33" s="9" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="14.5" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="14.5" customHeight="1">
       <c r="A35" s="9" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="14.5" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="14.5" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>341</v>
+        <v>107</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="14.5" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>121</v>
+        <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="14.5" customHeight="1">
       <c r="A39" s="9" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="14.5" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="14.5" customHeight="1">
       <c r="A41" s="9" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>129</v>
+        <v>341</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>96</v>
+    <row r="42" spans="1:3" ht="14.5" customHeight="1">
+      <c r="A42" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>61</v>
+    <row r="43" spans="1:3" ht="14.5" customHeight="1">
+      <c r="A43" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>305</v>
       </c>
     </row>
+    <row r="44" spans="1:3" ht="14.5" customHeight="1">
+      <c r="A44" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.5" customHeight="1">
+      <c r="A45" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -4869,17 +4971,15 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IW1048573"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.6640625" style="4" customWidth="1"/>
     <col min="2" max="3" width="15.5" style="4" customWidth="1"/>
@@ -4891,7 +4991,7 @@
     <col min="258" max="1025" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:257" s="39" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:257" s="39" customFormat="1" ht="27" customHeight="1">
       <c r="A1" s="36" t="s">
         <v>377</v>
       </c>
@@ -5148,7 +5248,7 @@
       <c r="IR1" s="37"/>
       <c r="IS1" s="37"/>
     </row>
-    <row r="2" spans="1:257" s="12" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:257" s="12" customFormat="1" ht="14.75" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -5403,7 +5503,7 @@
       <c r="IR2" s="4"/>
       <c r="IS2" s="4"/>
     </row>
-    <row r="3" spans="1:257" s="15" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:257" s="15" customFormat="1" ht="14.75" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>348</v>
       </c>
@@ -5662,7 +5762,7 @@
       <c r="IR3" s="14"/>
       <c r="IS3" s="14"/>
     </row>
-    <row r="4" spans="1:257" s="18" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:257" s="18" customFormat="1" ht="14.75" customHeight="1">
       <c r="A4" s="16" t="s">
         <v>350</v>
       </c>
@@ -5927,7 +6027,7 @@
       <c r="IR4" s="16"/>
       <c r="IS4" s="16"/>
     </row>
-    <row r="5" spans="1:257" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:257" ht="14.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>312</v>
       </c>
@@ -5947,7 +6047,7 @@
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:257" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:257" ht="14.5" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>329</v>
       </c>
@@ -5967,7 +6067,7 @@
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
     </row>
-    <row r="7" spans="1:257" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:257" ht="14.5" customHeight="1">
       <c r="D7" s="33"/>
       <c r="E7" s="4" t="s">
         <v>353</v>
@@ -5976,10 +6076,10 @@
         <v>353</v>
       </c>
     </row>
-    <row r="8" spans="1:257" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:257" ht="14.5" customHeight="1">
       <c r="D8" s="33"/>
     </row>
-    <row r="9" spans="1:257" s="15" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:257" s="15" customFormat="1" ht="14.5" customHeight="1">
       <c r="A9" s="20" t="s">
         <v>354</v>
       </c>
@@ -6242,7 +6342,7 @@
       <c r="IV9" s="14"/>
       <c r="IW9" s="14"/>
     </row>
-    <row r="10" spans="1:257" s="18" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:257" s="18" customFormat="1" ht="14.75" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>0</v>
       </c>
@@ -6515,7 +6615,7 @@
       <c r="IV10" s="16"/>
       <c r="IW10" s="16"/>
     </row>
-    <row r="11" spans="1:257" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:257" ht="14.75" customHeight="1">
       <c r="A11" s="23" t="s">
         <v>361</v>
       </c>
@@ -6546,7 +6646,7 @@
       <c r="IV11" s="4"/>
       <c r="IW11" s="4"/>
     </row>
-    <row r="12" spans="1:257" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:257" ht="14.75" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>365</v>
       </c>
@@ -6577,7 +6677,7 @@
       <c r="IV12" s="4"/>
       <c r="IW12" s="4"/>
     </row>
-    <row r="13" spans="1:257" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:257" ht="14.75" customHeight="1">
       <c r="A13" s="9" t="s">
         <v>352</v>
       </c>
@@ -6609,7 +6709,7 @@
       <c r="IV13" s="4"/>
       <c r="IW13" s="4"/>
     </row>
-    <row r="14" spans="1:257" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:257" ht="14.75" customHeight="1">
       <c r="A14" s="27" t="s">
         <v>371</v>
       </c>
@@ -6640,7 +6740,7 @@
       <c r="IV14" s="4"/>
       <c r="IW14" s="4"/>
     </row>
-    <row r="15" spans="1:257" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:257" ht="14.75" customHeight="1">
       <c r="A15" s="27" t="s">
         <v>374</v>
       </c>
@@ -6671,7 +6771,7 @@
       <c r="IV15" s="4"/>
       <c r="IW15" s="4"/>
     </row>
-    <row r="16" spans="1:257" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:257" ht="14.5" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -6682,15 +6782,16 @@
       <c r="IV16" s="4"/>
       <c r="IW16" s="4"/>
     </row>
-    <row r="17" spans="5:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:7" ht="14.75" customHeight="1">
       <c r="E17" s="23"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="1048571" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048572" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048571" ht="12.75" customHeight="1"/>
+    <row r="1048572" ht="12.75" customHeight="1"/>
+    <row r="1048573" ht="12.75" customHeight="1"/>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.51180555555555496" footer="0.25"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>